<commit_message>
zuletzt geändert von Annika
</commit_message>
<xml_diff>
--- a/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK.xlsx
+++ b/Meetings/Doku/Struktur_Doku - 2015.10.12 - EinkaufsApp Übersicht bis dato - AK.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dang\Desktop\EinkaufsApp\EinkaufsApp-Doku\Meetings\Doku\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="9735"/>
   </bookViews>
   <sheets>
-    <sheet name="alle" sheetId="3" r:id="rId1"/>
-    <sheet name="Skilltabelle" sheetId="9" r:id="rId2"/>
+    <sheet name="Skilltabelle" sheetId="9" r:id="rId1"/>
+    <sheet name="alle" sheetId="3" r:id="rId2"/>
     <sheet name="Design" sheetId="1" r:id="rId3"/>
     <sheet name="Dev" sheetId="2" r:id="rId4"/>
     <sheet name="Doku" sheetId="7" r:id="rId5"/>
@@ -25,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Telkos, Besprechungstermine'!$A$1:$C$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="122">
   <si>
     <t>Datum</t>
   </si>
@@ -1420,9 +1415,6 @@
     <t>ToDos an Developer (Eric, Daniel, Viktor, Florian) : http://www.1worldsync.com/web/de/download-center;jsessionid=a05PcEljkQCNSCFdmLEhj7Sr.nodeA anschauen</t>
   </si>
   <si>
-    <t>An Thoma und Annika</t>
-  </si>
-  <si>
     <t>*Struktur für Doku festlegen (was ist wichtig, was kann raus)
 *Liste anschauen und kommentieren</t>
   </si>
@@ -1502,6 +1494,61 @@
     <t>* Zwei Jahre Vertrieb
 * Tools LaTex
 * Grundlagen VBA</t>
+  </si>
+  <si>
+    <t>Annika Köstler</t>
+  </si>
+  <si>
+    <t>Michael Hein</t>
+  </si>
+  <si>
+    <t>Entwicklung</t>
+  </si>
+  <si>
+    <t>* Zwei Jahre Applikations Administration
+* Java Erfahrung
+*VBA Erfahrung
+*Skript Programmierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Zwei Jahre Controlling
+* Tools Latex
+*Grundkenntnisse VBA
+*Protokollierung von Meetings </t>
+  </si>
+  <si>
+    <t>Annika</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Huong</t>
+  </si>
+  <si>
+    <t>Definitionsphase
+Projektorganisation</t>
+  </si>
+  <si>
+    <t>Planungsphase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quellen </t>
+  </si>
+  <si>
+    <t>Definitionsphase
+Projektziel/ Sachziel</t>
+  </si>
+  <si>
+    <t>Defintionsphase
+Projektorganisation</t>
+  </si>
+  <si>
+    <t>Planungsphase
+Tools</t>
+  </si>
+  <si>
+    <t>An Thomas und Annika</t>
   </si>
 </sst>
 </file>
@@ -1628,7 +1675,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1674,7 +1721,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1742,9 +1788,13 @@
     <xf numFmtId="22" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1761,9 +1811,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1801,9 +1851,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1838,7 +1888,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1873,7 +1923,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2047,13 +2097,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="16" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,149 +2201,174 @@
     <col min="1" max="1" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="121.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
+      <c r="E1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A2" s="41">
         <v>42279.657638888886</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="43">
+      <c r="E2" s="25" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="42">
         <v>42283.412499999999</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="44">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="43">
         <v>42283.412499999999</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="44">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="43">
         <v>42283.412499999999</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="45">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="44">
         <v>42284.313888888886</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="46">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="45">
         <v>42284.405555555553</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42">
+    <row r="8" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41">
         <v>42284.418055555558</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42">
+      <c r="E8" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="41">
         <v>42287</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="21" customFormat="1" ht="330" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+    <row r="10" spans="1:7" s="48" customFormat="1" ht="330" x14ac:dyDescent="0.25">
+      <c r="A10" s="46">
         <v>42287</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>64</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="21" customFormat="1" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="28" t="s">
+      <c r="E10" s="49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="48" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="46"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="27" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="48">
+      <c r="E11" s="49" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="47">
         <v>42289.418055555558</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="39" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="42">
+      <c r="E12" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="41">
         <v>42290.511805555558</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="33" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="45">
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="44">
         <v>42291.345833333333</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2213,8 +2378,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="45">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="44">
         <v>42292.513888888891</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2224,8 +2389,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45">
+    <row r="16" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="44">
         <v>42293.595833333333</v>
       </c>
       <c r="B16" t="s">
@@ -2236,25 +2401,25 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="255" x14ac:dyDescent="0.25">
-      <c r="A17" s="45">
+      <c r="A17" s="44">
         <v>42296.447222222225</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="18" spans="1:3" ht="165" x14ac:dyDescent="0.25">
-      <c r="A18" s="45">
+      <c r="A18" s="44">
         <v>42297.324999999997</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2263,82 +2428,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" style="16" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="41" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>101</v>
-      </c>
-      <c r="D1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,10 +2444,12 @@
     <col min="1" max="1" width="15.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="101" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="3"/>
+    <col min="4" max="4" width="27.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2359,8 +2459,17 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>42283.475694444445</v>
       </c>
@@ -2371,18 +2480,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>42283.484722222223</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>42283.540277777778</v>
       </c>
@@ -2392,8 +2504,11 @@
       <c r="C4" s="6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D4" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>42283.627083333333</v>
       </c>
@@ -2404,7 +2519,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>42283.481249999997</v>
       </c>
@@ -2415,7 +2530,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>42284.464583333334</v>
       </c>
@@ -2425,8 +2540,11 @@
       <c r="C7" s="5" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>42285.359027777777</v>
       </c>
@@ -2437,7 +2555,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A9" s="19">
         <v>42288</v>
       </c>
@@ -2446,6 +2564,9 @@
       </c>
       <c r="C9" s="6" t="s">
         <v>79</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2456,13 +2577,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2470,9 +2591,10 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" style="16" customWidth="1"/>
     <col min="3" max="3" width="110.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2482,8 +2604,17 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42283.557638888888</v>
       </c>
@@ -2493,8 +2624,11 @@
       <c r="C2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42288</v>
       </c>
@@ -2504,8 +2638,11 @@
       <c r="C3" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+      <c r="D3" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>42289.911805555559</v>
       </c>
@@ -2515,8 +2652,11 @@
       <c r="C4" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="255" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>42292.5</v>
       </c>
@@ -2525,6 +2665,9 @@
       </c>
       <c r="C5" s="2" t="s">
         <v>83</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2534,10 +2677,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,9 +2688,21 @@
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>42283.731944444444</v>
       </c>
@@ -2557,9 +2712,12 @@
       <c r="C2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="38">
+      <c r="D2" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="37">
         <v>42287</v>
       </c>
       <c r="B3" t="s">
@@ -2568,8 +2726,9 @@
       <c r="C3" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>42292</v>
       </c>
@@ -2579,27 +2738,33 @@
       <c r="C4" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42293.525694444441</v>
       </c>
       <c r="B5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42296.622916666667</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2621,7 +2786,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2660,46 +2825,46 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="27"/>
+      <c r="C6" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>